<commit_message>
add new employee seed data
</commit_message>
<xml_diff>
--- a/backend/app/data/employee.xlsx
+++ b/backend/app/data/employee.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.varasteh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\APP\WebApp\backend\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926998F2-3CC8-458F-8B06-0C2EB9DACB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16B8367-D8F5-486F-A0B7-88F4CA7C5B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="10" sheetId="1" r:id="rId1"/>
+    <sheet name="employee" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'10'!$A$2:$D$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">employee!$A$2:$F$208</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="301">
   <si>
     <t>رديف</t>
   </si>
@@ -919,6 +919,21 @@
   </si>
   <si>
     <t>سرپرست</t>
+  </si>
+  <si>
+    <t>سرشیفت</t>
+  </si>
+  <si>
+    <t>M.Shekari</t>
+  </si>
+  <si>
+    <t>F.Mansourian</t>
+  </si>
+  <si>
+    <t>E.Najafi</t>
+  </si>
+  <si>
+    <t>M.Mehdizadeh</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1264,34 +1279,43 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1576,30 +1600,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M208"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="32" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1612,10 +1638,10 @@
       <c r="D2" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="30" t="s">
         <v>223</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -1625,7 +1651,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1638,10 +1664,10 @@
       <c r="D3" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>224</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1651,7 +1677,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -1664,10 +1690,10 @@
       <c r="D4" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="31" t="s">
         <v>225</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1677,7 +1703,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -1690,10 +1716,10 @@
       <c r="D5" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="31" t="s">
         <v>226</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1703,7 +1729,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1716,10 +1742,10 @@
       <c r="D6" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="31" t="s">
         <v>227</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1729,7 +1755,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -1742,14 +1768,18 @@
       <c r="D7" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>289</v>
       </c>
+      <c r="F7" s="31"/>
       <c r="L7" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="M7" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -1762,17 +1792,17 @@
       <c r="D8" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="31" t="s">
         <v>228</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A9" s="15">
         <v>7</v>
       </c>
@@ -1785,17 +1815,17 @@
       <c r="D9" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="31" t="s">
         <v>229</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>8</v>
       </c>
@@ -1808,14 +1838,15 @@
       <c r="D10" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E10" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F10" s="31"/>
       <c r="L10" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>9</v>
       </c>
@@ -1828,14 +1859,15 @@
       <c r="D11" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="22" t="s">
         <v>289</v>
       </c>
+      <c r="F11" s="31"/>
       <c r="L11" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>10</v>
       </c>
@@ -1848,17 +1880,17 @@
       <c r="D12" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="31" t="s">
         <v>230</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>11</v>
       </c>
@@ -1871,14 +1903,15 @@
       <c r="D13" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E13" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F13" s="31"/>
       <c r="L13" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>12</v>
       </c>
@@ -1891,14 +1924,15 @@
       <c r="D14" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E14" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F14" s="31"/>
       <c r="L14" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>13</v>
       </c>
@@ -1911,14 +1945,15 @@
       <c r="D15" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E15" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F15" s="31"/>
       <c r="L15" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>14</v>
       </c>
@@ -1931,14 +1966,15 @@
       <c r="D16" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E16" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F16" s="31"/>
       <c r="L16" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>15</v>
       </c>
@@ -1951,14 +1987,15 @@
       <c r="D17" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>290</v>
-      </c>
+      <c r="E17" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F17" s="31"/>
       <c r="L17" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>16</v>
       </c>
@@ -1971,11 +2008,12 @@
       <c r="D18" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E18" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A19" s="15">
         <v>17</v>
       </c>
@@ -1988,11 +2026,12 @@
       <c r="D19" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E19" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E19" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>18</v>
       </c>
@@ -2005,11 +2044,12 @@
       <c r="D20" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E20" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A21" s="15">
         <v>19</v>
       </c>
@@ -2022,14 +2062,14 @@
       <c r="D21" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="E21" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F21" s="31" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>20</v>
       </c>
@@ -2042,11 +2082,12 @@
       <c r="D22" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E22" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F22" s="31"/>
+    </row>
+    <row r="23" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>21</v>
       </c>
@@ -2059,11 +2100,12 @@
       <c r="D23" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E23" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F23" s="31"/>
+    </row>
+    <row r="24" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A24" s="15">
         <v>22</v>
       </c>
@@ -2076,11 +2118,14 @@
       <c r="D24" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E24" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A25" s="15">
         <v>23</v>
       </c>
@@ -2093,14 +2138,14 @@
       <c r="D25" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A26" s="15">
         <v>24</v>
       </c>
@@ -2113,11 +2158,12 @@
       <c r="D26" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E26" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A27" s="15">
         <v>25</v>
       </c>
@@ -2130,11 +2176,12 @@
       <c r="D27" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E27" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F27" s="31"/>
+    </row>
+    <row r="28" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A28" s="15">
         <v>26</v>
       </c>
@@ -2147,11 +2194,12 @@
       <c r="D28" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E28" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A29" s="15">
         <v>27</v>
       </c>
@@ -2164,11 +2212,12 @@
       <c r="D29" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E29" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F29" s="31"/>
+    </row>
+    <row r="30" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A30" s="15">
         <v>28</v>
       </c>
@@ -2181,11 +2230,12 @@
       <c r="D30" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E30" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F30" s="31"/>
+    </row>
+    <row r="31" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A31" s="15">
         <v>29</v>
       </c>
@@ -2198,11 +2248,12 @@
       <c r="D31" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E31" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="31"/>
+    </row>
+    <row r="32" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A32" s="15">
         <v>30</v>
       </c>
@@ -2215,14 +2266,14 @@
       <c r="D32" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="31" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A33" s="15">
         <v>31</v>
       </c>
@@ -2235,14 +2286,14 @@
       <c r="D33" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="31" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A34" s="15">
         <v>32</v>
       </c>
@@ -2255,11 +2306,12 @@
       <c r="D34" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E34" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E34" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F34" s="31"/>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A35" s="15">
         <v>33</v>
       </c>
@@ -2272,11 +2324,12 @@
       <c r="D35" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E35" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E35" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A36" s="15">
         <v>34</v>
       </c>
@@ -2289,11 +2342,12 @@
       <c r="D36" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E36" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F36" s="31"/>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A37" s="15">
         <v>35</v>
       </c>
@@ -2306,11 +2360,12 @@
       <c r="D37" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E37" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E37" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F37" s="31"/>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A38" s="15">
         <v>36</v>
       </c>
@@ -2323,11 +2378,12 @@
       <c r="D38" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E38" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E38" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F38" s="31"/>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A39" s="15">
         <v>37</v>
       </c>
@@ -2340,14 +2396,14 @@
       <c r="D39" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="31" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A40" s="15">
         <v>38</v>
       </c>
@@ -2360,11 +2416,12 @@
       <c r="D40" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E40" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E40" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F40" s="31"/>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A41" s="15">
         <v>39</v>
       </c>
@@ -2377,11 +2434,12 @@
       <c r="D41" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E41" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E41" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F41" s="31"/>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A42" s="15">
         <v>40</v>
       </c>
@@ -2394,11 +2452,14 @@
       <c r="D42" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E42" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A43" s="15">
         <v>41</v>
       </c>
@@ -2411,14 +2472,14 @@
       <c r="D43" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E43" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F43" s="3" t="s">
+      <c r="E43" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F43" s="31" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A44" s="15">
         <v>42</v>
       </c>
@@ -2431,11 +2492,12 @@
       <c r="D44" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E44" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E44" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F44" s="31"/>
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A45" s="15">
         <v>43</v>
       </c>
@@ -2448,11 +2510,12 @@
       <c r="D45" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E45" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E45" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A46" s="15">
         <v>44</v>
       </c>
@@ -2465,14 +2528,14 @@
       <c r="D46" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="31" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A47" s="15">
         <v>45</v>
       </c>
@@ -2485,11 +2548,12 @@
       <c r="D47" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E47" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E47" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A48" s="15">
         <v>46</v>
       </c>
@@ -2502,11 +2566,12 @@
       <c r="D48" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E48" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E48" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F48" s="31"/>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A49" s="15">
         <v>47</v>
       </c>
@@ -2519,11 +2584,12 @@
       <c r="D49" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E49" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E49" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F49" s="31"/>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A50" s="15">
         <v>48</v>
       </c>
@@ -2536,14 +2602,14 @@
       <c r="D50" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="31" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A51" s="15">
         <v>49</v>
       </c>
@@ -2556,11 +2622,12 @@
       <c r="D51" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E51" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A52" s="15">
         <v>50</v>
       </c>
@@ -2573,11 +2640,12 @@
       <c r="D52" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E52" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A53" s="15">
         <v>51</v>
       </c>
@@ -2590,14 +2658,14 @@
       <c r="D53" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="E53" s="24" t="s">
+      <c r="E53" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="31" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A54" s="15">
         <v>52</v>
       </c>
@@ -2610,11 +2678,12 @@
       <c r="D54" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E54" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E54" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A55" s="15">
         <v>53</v>
       </c>
@@ -2627,14 +2696,14 @@
       <c r="D55" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E55" s="26" t="s">
+      <c r="E55" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="31" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A56" s="15">
         <v>54</v>
       </c>
@@ -2647,14 +2716,14 @@
       <c r="D56" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E56" s="26" t="s">
+      <c r="E56" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F56" s="31" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A57" s="15">
         <v>55</v>
       </c>
@@ -2667,14 +2736,14 @@
       <c r="D57" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="26" t="s">
+      <c r="E57" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="31" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A58" s="15">
         <v>56</v>
       </c>
@@ -2687,11 +2756,12 @@
       <c r="D58" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E58" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E58" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F58" s="31"/>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A59" s="15">
         <v>57</v>
       </c>
@@ -2704,11 +2774,12 @@
       <c r="D59" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E59" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E59" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F59" s="31"/>
+    </row>
+    <row r="60" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A60" s="15">
         <v>58</v>
       </c>
@@ -2721,14 +2792,14 @@
       <c r="D60" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E60" s="24" t="s">
+      <c r="E60" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="31" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A61" s="15">
         <v>59</v>
       </c>
@@ -2741,11 +2812,12 @@
       <c r="D61" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E61" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E61" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F61" s="31"/>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A62" s="15">
         <v>60</v>
       </c>
@@ -2758,11 +2830,12 @@
       <c r="D62" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E62" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E62" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F62" s="31"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A63" s="15">
         <v>61</v>
       </c>
@@ -2775,11 +2848,12 @@
       <c r="D63" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E63" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E63" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F63" s="31"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A64" s="15">
         <v>62</v>
       </c>
@@ -2792,11 +2866,12 @@
       <c r="D64" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E64" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E64" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F64" s="31"/>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A65" s="15">
         <v>63</v>
       </c>
@@ -2809,11 +2884,12 @@
       <c r="D65" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E65" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E65" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F65" s="31"/>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A66" s="15">
         <v>64</v>
       </c>
@@ -2826,14 +2902,14 @@
       <c r="D66" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E66" s="24" t="s">
+      <c r="E66" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="31" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A67" s="15">
         <v>65</v>
       </c>
@@ -2846,11 +2922,12 @@
       <c r="D67" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E67" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E67" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F67" s="31"/>
+    </row>
+    <row r="68" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A68" s="15">
         <v>66</v>
       </c>
@@ -2863,14 +2940,14 @@
       <c r="D68" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E68" s="24" t="s">
+      <c r="E68" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="31" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A69" s="15">
         <v>67</v>
       </c>
@@ -2883,11 +2960,12 @@
       <c r="D69" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E69" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E69" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F69" s="31"/>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A70" s="15">
         <v>68</v>
       </c>
@@ -2900,11 +2978,12 @@
       <c r="D70" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E70" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E70" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F70" s="31"/>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A71" s="15">
         <v>69</v>
       </c>
@@ -2917,14 +2996,14 @@
       <c r="D71" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E71" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F71" s="3" t="s">
+      <c r="E71" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F71" s="31" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A72" s="15">
         <v>70</v>
       </c>
@@ -2937,11 +3016,12 @@
       <c r="D72" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E72" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E72" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F72" s="31"/>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A73" s="15">
         <v>71</v>
       </c>
@@ -2954,11 +3034,12 @@
       <c r="D73" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E73" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E73" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F73" s="31"/>
+    </row>
+    <row r="74" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A74" s="15">
         <v>72</v>
       </c>
@@ -2971,11 +3052,12 @@
       <c r="D74" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E74" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E74" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F74" s="31"/>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A75" s="15">
         <v>73</v>
       </c>
@@ -2988,11 +3070,12 @@
       <c r="D75" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E75" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F75" s="31"/>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A76" s="15">
         <v>74</v>
       </c>
@@ -3005,14 +3088,14 @@
       <c r="D76" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E76" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F76" s="31" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A77" s="15">
         <v>75</v>
       </c>
@@ -3025,14 +3108,14 @@
       <c r="D77" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E77" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F77" s="31" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A78" s="15">
         <v>76</v>
       </c>
@@ -3045,11 +3128,12 @@
       <c r="D78" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E78" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E78" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F78" s="31"/>
+    </row>
+    <row r="79" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A79" s="15">
         <v>77</v>
       </c>
@@ -3062,14 +3146,14 @@
       <c r="D79" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E79" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F79" s="31" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A80" s="15">
         <v>78</v>
       </c>
@@ -3082,11 +3166,12 @@
       <c r="D80" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E80" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E80" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F80" s="31"/>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A81" s="15">
         <v>79</v>
       </c>
@@ -3099,11 +3184,12 @@
       <c r="D81" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E81" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E81" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F81" s="31"/>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A82" s="15">
         <v>80</v>
       </c>
@@ -3116,11 +3202,12 @@
       <c r="D82" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E82" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E82" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" s="31"/>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A83" s="15">
         <v>81</v>
       </c>
@@ -3133,11 +3220,12 @@
       <c r="D83" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E83" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E83" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F83" s="31"/>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A84" s="15">
         <v>82</v>
       </c>
@@ -3150,14 +3238,14 @@
       <c r="D84" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E84" s="24" t="s">
+      <c r="E84" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="F84" s="31" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A85" s="15">
         <v>83</v>
       </c>
@@ -3170,11 +3258,12 @@
       <c r="D85" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E85" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E85" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F85" s="31"/>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A86" s="15">
         <v>84</v>
       </c>
@@ -3187,11 +3276,12 @@
       <c r="D86" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E86" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E86" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F86" s="31"/>
+    </row>
+    <row r="87" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A87" s="15">
         <v>85</v>
       </c>
@@ -3204,11 +3294,12 @@
       <c r="D87" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E87" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E87" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F87" s="31"/>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A88" s="15">
         <v>86</v>
       </c>
@@ -3221,11 +3312,12 @@
       <c r="D88" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E88" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E88" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F88" s="31"/>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A89" s="15">
         <v>87</v>
       </c>
@@ -3238,11 +3330,12 @@
       <c r="D89" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E89" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E89" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F89" s="31"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A90" s="15">
         <v>88</v>
       </c>
@@ -3255,11 +3348,12 @@
       <c r="D90" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E90" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E90" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F90" s="31"/>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A91" s="15">
         <v>89</v>
       </c>
@@ -3272,14 +3366,14 @@
       <c r="D91" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="E91" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="F91" s="3" t="s">
+      <c r="E91" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F91" s="31" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A92" s="15">
         <v>90</v>
       </c>
@@ -3292,14 +3386,14 @@
       <c r="D92" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E92" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F92" s="3" t="s">
+      <c r="E92" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F92" s="31" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A93" s="15">
         <v>91</v>
       </c>
@@ -3312,14 +3406,14 @@
       <c r="D93" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E93" s="25" t="s">
+      <c r="E93" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="F93" s="31" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A94" s="15">
         <v>92</v>
       </c>
@@ -3332,11 +3426,12 @@
       <c r="D94" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E94" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E94" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F94" s="31"/>
+    </row>
+    <row r="95" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A95" s="15">
         <v>93</v>
       </c>
@@ -3349,11 +3444,12 @@
       <c r="D95" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E95" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E95" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F95" s="31"/>
+    </row>
+    <row r="96" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A96" s="15">
         <v>94</v>
       </c>
@@ -3366,11 +3462,12 @@
       <c r="D96" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E96" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E96" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F96" s="31"/>
+    </row>
+    <row r="97" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A97" s="15">
         <v>95</v>
       </c>
@@ -3383,11 +3480,12 @@
       <c r="D97" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E97" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E97" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F97" s="31"/>
+    </row>
+    <row r="98" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A98" s="15">
         <v>96</v>
       </c>
@@ -3400,11 +3498,12 @@
       <c r="D98" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E98" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E98" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F98" s="31"/>
+    </row>
+    <row r="99" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A99" s="15">
         <v>97</v>
       </c>
@@ -3417,11 +3516,12 @@
       <c r="D99" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E99" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E99" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F99" s="31"/>
+    </row>
+    <row r="100" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A100" s="15">
         <v>98</v>
       </c>
@@ -3434,11 +3534,12 @@
       <c r="D100" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E100" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E100" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F100" s="31"/>
+    </row>
+    <row r="101" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A101" s="15">
         <v>99</v>
       </c>
@@ -3451,14 +3552,14 @@
       <c r="D101" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E101" s="24" t="s">
+      <c r="E101" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F101" s="31" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A102" s="15">
         <v>100</v>
       </c>
@@ -3471,11 +3572,12 @@
       <c r="D102" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E102" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E102" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F102" s="31"/>
+    </row>
+    <row r="103" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A103" s="15">
         <v>101</v>
       </c>
@@ -3488,14 +3590,14 @@
       <c r="D103" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E103" s="24" t="s">
+      <c r="E103" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F103" s="31" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A104" s="15">
         <v>102</v>
       </c>
@@ -3508,14 +3610,14 @@
       <c r="D104" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E104" s="24" t="s">
+      <c r="E104" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="F104" s="31" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A105" s="15">
         <v>103</v>
       </c>
@@ -3528,11 +3630,12 @@
       <c r="D105" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E105" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E105" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F105" s="31"/>
+    </row>
+    <row r="106" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A106" s="15">
         <v>104</v>
       </c>
@@ -3545,14 +3648,14 @@
       <c r="D106" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E106" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F106" s="3" t="s">
+      <c r="E106" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F106" s="31" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A107" s="15">
         <v>105</v>
       </c>
@@ -3565,14 +3668,14 @@
       <c r="D107" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E107" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F107" s="3" t="s">
+      <c r="E107" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F107" s="31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="108" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A108" s="15">
         <v>106</v>
       </c>
@@ -3585,11 +3688,12 @@
       <c r="D108" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E108" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E108" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F108" s="31"/>
+    </row>
+    <row r="109" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A109" s="15">
         <v>107</v>
       </c>
@@ -3602,14 +3706,14 @@
       <c r="D109" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E109" s="25" t="s">
+      <c r="E109" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="F109" s="3" t="s">
+      <c r="F109" s="31" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="110" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A110" s="15">
         <v>108</v>
       </c>
@@ -3622,14 +3726,14 @@
       <c r="D110" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E110" s="25" t="s">
+      <c r="E110" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="F110" s="3" t="s">
+      <c r="F110" s="31" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A111" s="15">
         <v>109</v>
       </c>
@@ -3642,11 +3746,12 @@
       <c r="D111" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E111" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E111" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F111" s="31"/>
+    </row>
+    <row r="112" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A112" s="15">
         <v>110</v>
       </c>
@@ -3659,11 +3764,12 @@
       <c r="D112" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E112" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E112" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F112" s="31"/>
+    </row>
+    <row r="113" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A113" s="15">
         <v>111</v>
       </c>
@@ -3676,11 +3782,12 @@
       <c r="D113" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E113" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E113" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F113" s="31"/>
+    </row>
+    <row r="114" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A114" s="15">
         <v>112</v>
       </c>
@@ -3693,11 +3800,12 @@
       <c r="D114" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E114" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E114" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F114" s="31"/>
+    </row>
+    <row r="115" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A115" s="15">
         <v>113</v>
       </c>
@@ -3710,11 +3818,12 @@
       <c r="D115" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E115" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E115" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F115" s="31"/>
+    </row>
+    <row r="116" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A116" s="15">
         <v>114</v>
       </c>
@@ -3727,14 +3836,14 @@
       <c r="D116" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E116" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F116" s="3" t="s">
+      <c r="E116" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F116" s="31" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="117" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A117" s="15">
         <v>115</v>
       </c>
@@ -3747,11 +3856,12 @@
       <c r="D117" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E117" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E117" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F117" s="31"/>
+    </row>
+    <row r="118" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A118" s="15">
         <v>116</v>
       </c>
@@ -3764,14 +3874,14 @@
       <c r="D118" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E118" s="25" t="s">
+      <c r="E118" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="F118" s="3" t="s">
+      <c r="F118" s="31" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="119" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A119" s="15">
         <v>117</v>
       </c>
@@ -3784,14 +3894,14 @@
       <c r="D119" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E119" s="25" t="s">
+      <c r="E119" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="F119" s="3" t="s">
+      <c r="F119" s="31" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="120" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A120" s="15">
         <v>118</v>
       </c>
@@ -3804,11 +3914,12 @@
       <c r="D120" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E120" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E120" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F120" s="31"/>
+    </row>
+    <row r="121" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A121" s="15">
         <v>119</v>
       </c>
@@ -3821,11 +3932,12 @@
       <c r="D121" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E121" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E121" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F121" s="31"/>
+    </row>
+    <row r="122" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A122" s="15">
         <v>120</v>
       </c>
@@ -3838,11 +3950,12 @@
       <c r="D122" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E122" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E122" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F122" s="31"/>
+    </row>
+    <row r="123" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A123" s="15">
         <v>121</v>
       </c>
@@ -3855,11 +3968,12 @@
       <c r="D123" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E123" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E123" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F123" s="31"/>
+    </row>
+    <row r="124" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A124" s="15">
         <v>122</v>
       </c>
@@ -3872,11 +3986,12 @@
       <c r="D124" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E124" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E124" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F124" s="31"/>
+    </row>
+    <row r="125" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A125" s="15">
         <v>123</v>
       </c>
@@ -3889,11 +4004,12 @@
       <c r="D125" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E125" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E125" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F125" s="31"/>
+    </row>
+    <row r="126" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A126" s="15">
         <v>124</v>
       </c>
@@ -3906,14 +4022,14 @@
       <c r="D126" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="E126" s="27" t="s">
+      <c r="E126" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="F126" s="3" t="s">
+      <c r="F126" s="31" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="127" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A127" s="15">
         <v>125</v>
       </c>
@@ -3926,11 +4042,12 @@
       <c r="D127" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E127" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E127" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F127" s="31"/>
+    </row>
+    <row r="128" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A128" s="15">
         <v>126</v>
       </c>
@@ -3943,11 +4060,14 @@
       <c r="D128" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="E128" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E128" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F128" s="31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A129" s="15">
         <v>127</v>
       </c>
@@ -3960,11 +4080,12 @@
       <c r="D129" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E129" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E129" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F129" s="31"/>
+    </row>
+    <row r="130" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A130" s="15">
         <v>128</v>
       </c>
@@ -3977,14 +4098,14 @@
       <c r="D130" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E130" s="25" t="s">
+      <c r="E130" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="F130" s="3" t="s">
+      <c r="F130" s="31" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="131" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A131" s="15">
         <v>129</v>
       </c>
@@ -3997,11 +4118,12 @@
       <c r="D131" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E131" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E131" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F131" s="31"/>
+    </row>
+    <row r="132" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A132" s="15">
         <v>130</v>
       </c>
@@ -4014,11 +4136,12 @@
       <c r="D132" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E132" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E132" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F132" s="31"/>
+    </row>
+    <row r="133" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A133" s="15">
         <v>131</v>
       </c>
@@ -4031,11 +4154,12 @@
       <c r="D133" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E133" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E133" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F133" s="31"/>
+    </row>
+    <row r="134" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A134" s="15">
         <v>132</v>
       </c>
@@ -4048,14 +4172,14 @@
       <c r="D134" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E134" s="25" t="s">
+      <c r="E134" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="F134" s="3" t="s">
+      <c r="F134" s="31" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A135" s="15">
         <v>133</v>
       </c>
@@ -4068,11 +4192,12 @@
       <c r="D135" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E135" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E135" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F135" s="31"/>
+    </row>
+    <row r="136" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A136" s="15">
         <v>134</v>
       </c>
@@ -4085,11 +4210,12 @@
       <c r="D136" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E136" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E136" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F136" s="31"/>
+    </row>
+    <row r="137" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A137" s="15">
         <v>135</v>
       </c>
@@ -4102,14 +4228,14 @@
       <c r="D137" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E137" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F137" s="3" t="s">
+      <c r="E137" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F137" s="31" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="138" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A138" s="15">
         <v>136</v>
       </c>
@@ -4122,11 +4248,12 @@
       <c r="D138" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E138" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E138" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F138" s="31"/>
+    </row>
+    <row r="139" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A139" s="15">
         <v>137</v>
       </c>
@@ -4139,11 +4266,12 @@
       <c r="D139" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E139" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E139" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F139" s="31"/>
+    </row>
+    <row r="140" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A140" s="15">
         <v>138</v>
       </c>
@@ -4156,14 +4284,14 @@
       <c r="D140" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E140" s="24" t="s">
+      <c r="E140" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="F140" s="3" t="s">
+      <c r="F140" s="31" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="141" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A141" s="15">
         <v>139</v>
       </c>
@@ -4176,11 +4304,12 @@
       <c r="D141" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E141" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E141" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="F141" s="31"/>
+    </row>
+    <row r="142" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A142" s="15">
         <v>140</v>
       </c>
@@ -4193,14 +4322,14 @@
       <c r="D142" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E142" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="F142" s="3" t="s">
+      <c r="E142" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F142" s="31" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="143" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A143" s="15">
         <v>141</v>
       </c>
@@ -4213,14 +4342,14 @@
       <c r="D143" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="E143" s="25" t="s">
+      <c r="E143" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="F143" s="3" t="s">
+      <c r="F143" s="31" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="144" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A144" s="15">
         <v>142</v>
       </c>
@@ -4233,14 +4362,14 @@
       <c r="D144" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E144" s="24" t="s">
+      <c r="E144" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="F144" s="3" t="s">
+      <c r="F144" s="31" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="145" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A145" s="15">
         <v>143</v>
       </c>
@@ -4253,11 +4382,12 @@
       <c r="D145" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="E145" s="24" t="s">
+      <c r="E145" s="22" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="F145" s="31"/>
+    </row>
+    <row r="146" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A146" s="15">
         <v>144</v>
       </c>
@@ -4270,14 +4400,14 @@
       <c r="D146" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="E146" s="25" t="s">
+      <c r="E146" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="F146" s="3" t="s">
+      <c r="F146" s="31" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="147" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A147" s="15">
         <v>145</v>
       </c>
@@ -4290,11 +4420,12 @@
       <c r="D147" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E147" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E147" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F147" s="31"/>
+    </row>
+    <row r="148" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A148" s="15">
         <v>146</v>
       </c>
@@ -4307,14 +4438,14 @@
       <c r="D148" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E148" s="25" t="s">
+      <c r="E148" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="F148" s="3" t="s">
+      <c r="F148" s="31" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="149" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A149" s="15">
         <v>147</v>
       </c>
@@ -4327,11 +4458,12 @@
       <c r="D149" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E149" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E149" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F149" s="31"/>
+    </row>
+    <row r="150" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A150" s="15">
         <v>148</v>
       </c>
@@ -4344,11 +4476,12 @@
       <c r="D150" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E150" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E150" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F150" s="31"/>
+    </row>
+    <row r="151" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A151" s="15">
         <v>149</v>
       </c>
@@ -4361,11 +4494,12 @@
       <c r="D151" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E151" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E151" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F151" s="31"/>
+    </row>
+    <row r="152" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A152" s="15">
         <v>150</v>
       </c>
@@ -4378,11 +4512,12 @@
       <c r="D152" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E152" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E152" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F152" s="31"/>
+    </row>
+    <row r="153" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A153" s="15">
         <v>151</v>
       </c>
@@ -4395,11 +4530,12 @@
       <c r="D153" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E153" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E153" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F153" s="31"/>
+    </row>
+    <row r="154" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A154" s="15">
         <v>152</v>
       </c>
@@ -4412,11 +4548,12 @@
       <c r="D154" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E154" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E154" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F154" s="31"/>
+    </row>
+    <row r="155" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A155" s="15">
         <v>153</v>
       </c>
@@ -4429,14 +4566,14 @@
       <c r="D155" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E155" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F155" s="3" t="s">
+      <c r="E155" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F155" s="31" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A156" s="15">
         <v>154</v>
       </c>
@@ -4449,11 +4586,12 @@
       <c r="D156" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E156" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E156" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F156" s="31"/>
+    </row>
+    <row r="157" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A157" s="15">
         <v>155</v>
       </c>
@@ -4466,11 +4604,12 @@
       <c r="D157" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E157" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E157" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F157" s="31"/>
+    </row>
+    <row r="158" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A158" s="15">
         <v>156</v>
       </c>
@@ -4483,11 +4622,12 @@
       <c r="D158" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E158" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E158" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F158" s="31"/>
+    </row>
+    <row r="159" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A159" s="15">
         <v>157</v>
       </c>
@@ -4500,11 +4640,12 @@
       <c r="D159" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E159" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E159" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F159" s="31"/>
+    </row>
+    <row r="160" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A160" s="15">
         <v>158</v>
       </c>
@@ -4517,11 +4658,12 @@
       <c r="D160" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E160" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E160" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F160" s="31"/>
+    </row>
+    <row r="161" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A161" s="15">
         <v>159</v>
       </c>
@@ -4534,11 +4676,12 @@
       <c r="D161" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E161" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E161" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F161" s="31"/>
+    </row>
+    <row r="162" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A162" s="15">
         <v>160</v>
       </c>
@@ -4551,11 +4694,12 @@
       <c r="D162" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E162" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E162" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F162" s="31"/>
+    </row>
+    <row r="163" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A163" s="15">
         <v>161</v>
       </c>
@@ -4568,11 +4712,12 @@
       <c r="D163" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E163" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E163" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F163" s="31"/>
+    </row>
+    <row r="164" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A164" s="15">
         <v>162</v>
       </c>
@@ -4585,11 +4730,12 @@
       <c r="D164" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E164" s="25" t="s">
+      <c r="E164" s="23" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="F164" s="31"/>
+    </row>
+    <row r="165" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A165" s="15">
         <v>163</v>
       </c>
@@ -4602,14 +4748,14 @@
       <c r="D165" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="E165" s="25" t="s">
+      <c r="E165" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="F165" s="3" t="s">
+      <c r="F165" s="31" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="166" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A166" s="15">
         <v>164</v>
       </c>
@@ -4622,14 +4768,14 @@
       <c r="D166" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E166" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="F166" s="3" t="s">
+      <c r="E166" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F166" s="31" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="167" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A167" s="15">
         <v>165</v>
       </c>
@@ -4642,11 +4788,12 @@
       <c r="D167" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E167" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E167" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F167" s="31"/>
+    </row>
+    <row r="168" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A168" s="15">
         <v>166</v>
       </c>
@@ -4657,16 +4804,16 @@
         <v>168</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="E168" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="E168" s="23" t="s">
         <v>287</v>
       </c>
-      <c r="F168" s="3" t="s">
+      <c r="F168" s="31" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="169" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A169" s="15">
         <v>167</v>
       </c>
@@ -4679,11 +4826,12 @@
       <c r="D169" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E169" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E169" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F169" s="31"/>
+    </row>
+    <row r="170" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A170" s="15">
         <v>168</v>
       </c>
@@ -4696,11 +4844,12 @@
       <c r="D170" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="E170" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E170" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F170" s="31"/>
+    </row>
+    <row r="171" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A171" s="15">
         <v>169</v>
       </c>
@@ -4713,11 +4862,14 @@
       <c r="D171" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="E171" s="24" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E171" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F171" s="31" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A172" s="15">
         <v>170</v>
       </c>
@@ -4730,11 +4882,12 @@
       <c r="D172" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E172" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E172" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F172" s="31"/>
+    </row>
+    <row r="173" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A173" s="15">
         <v>171</v>
       </c>
@@ -4747,11 +4900,12 @@
       <c r="D173" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E173" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" s="3" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.2">
+      <c r="E173" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F173" s="31"/>
+    </row>
+    <row r="174" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A174" s="15">
         <v>172</v>
       </c>
@@ -4764,11 +4918,12 @@
       <c r="D174" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E174" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E174" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="F174" s="31"/>
+    </row>
+    <row r="175" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A175" s="15">
         <v>173</v>
       </c>
@@ -4781,14 +4936,14 @@
       <c r="D175" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E175" s="28" t="s">
+      <c r="E175" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="F175" s="3" t="s">
+      <c r="F175" s="31" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="176" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A176" s="15">
         <v>174</v>
       </c>
@@ -4801,11 +4956,12 @@
       <c r="D176" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E176" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E176" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F176" s="31"/>
+    </row>
+    <row r="177" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A177" s="15">
         <v>175</v>
       </c>
@@ -4818,11 +4974,12 @@
       <c r="D177" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E177" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E177" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F177" s="31"/>
+    </row>
+    <row r="178" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A178" s="15">
         <v>176</v>
       </c>
@@ -4835,11 +4992,12 @@
       <c r="D178" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E178" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E178" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F178" s="31"/>
+    </row>
+    <row r="179" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A179" s="15">
         <v>177</v>
       </c>
@@ -4852,14 +5010,14 @@
       <c r="D179" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E179" s="28" t="s">
-        <v>295</v>
-      </c>
-      <c r="F179" s="3" t="s">
+      <c r="E179" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F179" s="31" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="180" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A180" s="15">
         <v>178</v>
       </c>
@@ -4872,11 +5030,12 @@
       <c r="D180" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E180" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E180" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F180" s="31"/>
+    </row>
+    <row r="181" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A181" s="15">
         <v>179</v>
       </c>
@@ -4889,11 +5048,12 @@
       <c r="D181" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E181" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E181" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F181" s="31"/>
+    </row>
+    <row r="182" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A182" s="15">
         <v>180</v>
       </c>
@@ -4906,11 +5066,12 @@
       <c r="D182" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E182" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E182" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F182" s="31"/>
+    </row>
+    <row r="183" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A183" s="15">
         <v>181</v>
       </c>
@@ -4923,11 +5084,12 @@
       <c r="D183" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E183" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E183" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F183" s="31"/>
+    </row>
+    <row r="184" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A184" s="15">
         <v>182</v>
       </c>
@@ -4940,11 +5102,12 @@
       <c r="D184" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E184" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E184" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F184" s="31"/>
+    </row>
+    <row r="185" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A185" s="15">
         <v>183</v>
       </c>
@@ -4957,14 +5120,14 @@
       <c r="D185" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E185" s="28" t="s">
+      <c r="E185" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="F185" s="3" t="s">
+      <c r="F185" s="31" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="186" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A186" s="15">
         <v>184</v>
       </c>
@@ -4977,11 +5140,12 @@
       <c r="D186" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E186" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E186" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F186" s="31"/>
+    </row>
+    <row r="187" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A187" s="15">
         <v>185</v>
       </c>
@@ -4994,11 +5158,12 @@
       <c r="D187" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E187" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E187" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F187" s="31"/>
+    </row>
+    <row r="188" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A188" s="15">
         <v>186</v>
       </c>
@@ -5011,14 +5176,14 @@
       <c r="D188" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E188" s="28" t="s">
+      <c r="E188" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="F188" s="3" t="s">
+      <c r="F188" s="31" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="189" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A189" s="15">
         <v>187</v>
       </c>
@@ -5031,11 +5196,12 @@
       <c r="D189" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E189" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E189" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F189" s="31"/>
+    </row>
+    <row r="190" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A190" s="15">
         <v>188</v>
       </c>
@@ -5048,11 +5214,12 @@
       <c r="D190" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E190" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E190" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F190" s="31"/>
+    </row>
+    <row r="191" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A191" s="15">
         <v>189</v>
       </c>
@@ -5065,11 +5232,12 @@
       <c r="D191" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E191" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E191" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F191" s="31"/>
+    </row>
+    <row r="192" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A192" s="15">
         <v>190</v>
       </c>
@@ -5082,11 +5250,12 @@
       <c r="D192" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E192" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E192" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F192" s="31"/>
+    </row>
+    <row r="193" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A193" s="15">
         <v>191</v>
       </c>
@@ -5099,11 +5268,12 @@
       <c r="D193" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E193" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E193" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F193" s="31"/>
+    </row>
+    <row r="194" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A194" s="15">
         <v>192</v>
       </c>
@@ -5116,11 +5286,12 @@
       <c r="D194" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E194" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E194" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F194" s="31"/>
+    </row>
+    <row r="195" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A195" s="15">
         <v>193</v>
       </c>
@@ -5133,11 +5304,12 @@
       <c r="D195" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E195" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E195" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F195" s="31"/>
+    </row>
+    <row r="196" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A196" s="15">
         <v>194</v>
       </c>
@@ -5150,11 +5322,12 @@
       <c r="D196" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E196" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E196" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F196" s="31"/>
+    </row>
+    <row r="197" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A197" s="15">
         <v>195</v>
       </c>
@@ -5167,11 +5340,12 @@
       <c r="D197" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E197" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E197" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F197" s="31"/>
+    </row>
+    <row r="198" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A198" s="15">
         <v>196</v>
       </c>
@@ -5184,11 +5358,12 @@
       <c r="D198" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E198" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E198" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F198" s="31"/>
+    </row>
+    <row r="199" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A199" s="15">
         <v>197</v>
       </c>
@@ -5201,14 +5376,14 @@
       <c r="D199" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E199" s="28" t="s">
+      <c r="E199" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="F199" s="3" t="s">
+      <c r="F199" s="31" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="200" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A200" s="15">
         <v>198</v>
       </c>
@@ -5221,11 +5396,12 @@
       <c r="D200" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E200" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E200" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F200" s="31"/>
+    </row>
+    <row r="201" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A201" s="15">
         <v>199</v>
       </c>
@@ -5238,14 +5414,14 @@
       <c r="D201" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E201" s="28" t="s">
+      <c r="E201" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="F201" s="3" t="s">
+      <c r="F201" s="31" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="202" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A202" s="15">
         <v>200</v>
       </c>
@@ -5258,14 +5434,14 @@
       <c r="D202" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E202" s="28" t="s">
+      <c r="E202" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="F202" s="3" t="s">
+      <c r="F202" s="31" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="203" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A203" s="15">
         <v>201</v>
       </c>
@@ -5278,11 +5454,12 @@
       <c r="D203" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E203" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E203" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F203" s="31"/>
+    </row>
+    <row r="204" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A204" s="15">
         <v>202</v>
       </c>
@@ -5295,11 +5472,12 @@
       <c r="D204" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E204" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E204" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F204" s="31"/>
+    </row>
+    <row r="205" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A205" s="15">
         <v>203</v>
       </c>
@@ -5312,11 +5490,12 @@
       <c r="D205" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E205" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" s="3" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.2">
+      <c r="E205" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F205" s="31"/>
+    </row>
+    <row r="206" spans="1:6" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A206" s="15">
         <v>204</v>
       </c>
@@ -5329,11 +5508,12 @@
       <c r="D206" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="E206" s="28" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="E206" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="F206" s="31"/>
+    </row>
+    <row r="207" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="15">
         <v>205</v>
       </c>
@@ -5346,14 +5526,14 @@
       <c r="D207" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="E207" s="29" t="s">
+      <c r="E207" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="F207" s="2" t="s">
+      <c r="F207" s="32" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="17">
         <v>206</v>
       </c>
@@ -5366,21 +5546,24 @@
       <c r="D208" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="E208" s="29" t="s">
+      <c r="E208" s="27" t="s">
         <v>287</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D206" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:F208" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{664C3659-DF2A-4518-9DD8-84B4A4D7DAEB}">
       <formula1>$L$2:$L$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{5104F684-2E3D-425B-8639-DA8BBF4BB60A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E44:E90 E167:E170 E172:E178 E180:E1048576 E108:E115 E117:E127 E143:E154 E129:E136 E138:E141 E4:E23 E25:E41 E93:E105 E156:E165 E1" xr:uid="{5104F684-2E3D-425B-8639-DA8BBF4BB60A}">
       <formula1>$M$2:$M$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 E116 E155 E179 E171 E128 E91:E92 E137 E142 E24 E42:E43 E106:E107 E166" xr:uid="{F8CCF1C6-924A-4D2F-B599-B32485D6F8C8}">
+      <formula1>$M$2:$M$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>